<commit_message>
Actualizacion del cronograma 29/12/2020
</commit_message>
<xml_diff>
--- a/Desarrollo/comparape/SCPPN_CP.xlsx
+++ b/Desarrollo/comparape/SCPPN_CP.xlsx
@@ -194,7 +194,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +217,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -327,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -418,6 +424,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,7 +652,7 @@
   <dimension ref="B1:J997"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -784,23 +800,23 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="41">
         <v>44193</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="42">
         <v>1</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="41">
         <v>44194</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="26">
-        <v>0</v>
+      <c r="G10" s="43">
+        <v>1</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="27"/>

</xml_diff>

<commit_message>
Actualización del cronograma 30/12/2020
</commit_message>
<xml_diff>
--- a/Desarrollo/comparape/SCPPN_CP.xlsx
+++ b/Desarrollo/comparape/SCPPN_CP.xlsx
@@ -209,12 +209,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
@@ -223,6 +217,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -400,11 +400,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -416,6 +413,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -424,16 +434,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,7 +652,7 @@
   <dimension ref="B1:J997"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -674,34 +674,34 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
     </row>
     <row r="3" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
     </row>
     <row r="4" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -800,58 +800,58 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10" s="36">
         <v>44193</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="37">
         <v>1</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="36">
         <v>44194</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="38">
         <v>1</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="27"/>
     </row>
     <row r="11" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="36">
         <v>44195</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="37">
         <v>1</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="36">
         <v>44195</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="26">
-        <v>0</v>
+      <c r="G11" s="38">
+        <v>1</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="27"/>
     </row>
     <row r="12" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="29">
         <v>44193</v>
       </c>
       <c r="D12" s="25"/>
-      <c r="E12" s="30">
+      <c r="E12" s="29">
         <v>44195</v>
       </c>
       <c r="F12" s="25"/>
@@ -860,7 +860,7 @@
       </c>
     </row>
     <row r="13" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="23">
@@ -869,7 +869,7 @@
       <c r="D13" s="25">
         <v>5</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="31">
         <v>44197</v>
       </c>
       <c r="F13" s="25" t="s">
@@ -881,7 +881,7 @@
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="32" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="23">
@@ -890,7 +890,7 @@
       <c r="D14" s="25">
         <v>5</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="31">
         <v>44197</v>
       </c>
       <c r="F14" s="25" t="s">
@@ -902,16 +902,16 @@
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="31">
         <v>44197</v>
       </c>
       <c r="D15" s="25">
         <v>3</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="31">
         <v>44198</v>
       </c>
       <c r="F15" s="24" t="s">
@@ -923,7 +923,7 @@
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="32" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="23">
@@ -944,14 +944,14 @@
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="29">
         <v>44196</v>
       </c>
       <c r="D17" s="25"/>
-      <c r="E17" s="30">
+      <c r="E17" s="29">
         <v>44198</v>
       </c>
       <c r="F17" s="25"/>
@@ -960,16 +960,16 @@
       </c>
     </row>
     <row r="18" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="31">
         <v>44199</v>
       </c>
       <c r="D18" s="25">
         <v>4</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="31">
         <v>44200</v>
       </c>
       <c r="F18" s="25" t="s">
@@ -984,13 +984,13 @@
       <c r="B19" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="31">
         <v>44199</v>
       </c>
       <c r="D19" s="25">
         <v>24</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="31">
         <v>44200</v>
       </c>
       <c r="F19" s="24" t="s">
@@ -1002,16 +1002,16 @@
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="31">
         <v>44200</v>
       </c>
       <c r="D20" s="25">
         <v>24</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="31">
         <v>44201</v>
       </c>
       <c r="F20" s="24" t="s">
@@ -1026,13 +1026,13 @@
       <c r="B21" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="31">
         <v>44200</v>
       </c>
       <c r="D21" s="25">
         <v>24</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="31">
         <v>44200</v>
       </c>
       <c r="F21" s="25" t="s">
@@ -1047,13 +1047,13 @@
       <c r="B22" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="31">
         <v>44201</v>
       </c>
       <c r="D22" s="25">
         <v>24</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="31">
         <v>44201</v>
       </c>
       <c r="F22" s="25" t="s">
@@ -1065,14 +1065,14 @@
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="30">
+      <c r="C23" s="29">
         <v>44199</v>
       </c>
       <c r="D23" s="25"/>
-      <c r="E23" s="30">
+      <c r="E23" s="29">
         <v>44201</v>
       </c>
       <c r="F23" s="25"/>
@@ -1084,13 +1084,13 @@
       <c r="B24" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="31">
         <v>44199</v>
       </c>
       <c r="D24" s="24">
         <v>1</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="31">
         <v>44199</v>
       </c>
       <c r="F24" s="25" t="s">
@@ -1105,13 +1105,13 @@
       <c r="B25" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="31">
         <v>44200</v>
       </c>
       <c r="D25" s="24">
         <v>1</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="31">
         <v>44200</v>
       </c>
       <c r="F25" s="25" t="s">
@@ -1123,7 +1123,7 @@
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="34" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="23">
@@ -1144,14 +1144,14 @@
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="30">
+      <c r="C27" s="29">
         <v>44202</v>
       </c>
       <c r="D27" s="25"/>
-      <c r="E27" s="30">
+      <c r="E27" s="29">
         <v>44204</v>
       </c>
       <c r="F27" s="25"/>

</xml_diff>

<commit_message>
Actualización del cronograma 31/12/2020
</commit_message>
<xml_diff>
--- a/Desarrollo/comparape/SCPPN_CP.xlsx
+++ b/Desarrollo/comparape/SCPPN_CP.xlsx
@@ -194,7 +194,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,6 +223,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -333,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -404,7 +410,6 @@
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -434,6 +439,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,7 +665,7 @@
   <dimension ref="B1:J997"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -674,34 +687,34 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
     </row>
     <row r="3" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -800,88 +813,88 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="35">
         <v>44193</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="36">
         <v>1</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="35">
         <v>44194</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="37">
         <v>1</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="27"/>
     </row>
     <row r="11" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="35">
         <v>44195</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="36">
         <v>1</v>
       </c>
-      <c r="E11" s="36">
+      <c r="E11" s="35">
         <v>44195</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="37">
         <v>1</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="27"/>
     </row>
     <row r="12" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="44">
         <v>44193</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="29">
+      <c r="D12" s="36"/>
+      <c r="E12" s="44">
         <v>44195</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26">
-        <v>0</v>
+      <c r="F12" s="36"/>
+      <c r="G12" s="37">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="35">
         <v>44196</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="36">
         <v>5</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E13" s="46">
         <v>44197</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="26">
-        <v>0</v>
+      <c r="G13" s="37">
+        <v>1</v>
       </c>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="31" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="23">
@@ -890,7 +903,7 @@
       <c r="D14" s="25">
         <v>5</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="30">
         <v>44197</v>
       </c>
       <c r="F14" s="25" t="s">
@@ -902,16 +915,16 @@
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="30">
         <v>44197</v>
       </c>
       <c r="D15" s="25">
         <v>3</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="30">
         <v>44198</v>
       </c>
       <c r="F15" s="24" t="s">
@@ -923,7 +936,7 @@
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="31" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="23">
@@ -960,16 +973,16 @@
       </c>
     </row>
     <row r="18" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="31">
+      <c r="C18" s="30">
         <v>44199</v>
       </c>
       <c r="D18" s="25">
         <v>4</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="30">
         <v>44200</v>
       </c>
       <c r="F18" s="25" t="s">
@@ -984,13 +997,13 @@
       <c r="B19" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="30">
         <v>44199</v>
       </c>
       <c r="D19" s="25">
         <v>24</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="30">
         <v>44200</v>
       </c>
       <c r="F19" s="24" t="s">
@@ -1002,16 +1015,16 @@
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="31">
+      <c r="C20" s="30">
         <v>44200</v>
       </c>
       <c r="D20" s="25">
         <v>24</v>
       </c>
-      <c r="E20" s="31">
+      <c r="E20" s="30">
         <v>44201</v>
       </c>
       <c r="F20" s="24" t="s">
@@ -1026,13 +1039,13 @@
       <c r="B21" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="30">
         <v>44200</v>
       </c>
       <c r="D21" s="25">
         <v>24</v>
       </c>
-      <c r="E21" s="31">
+      <c r="E21" s="30">
         <v>44200</v>
       </c>
       <c r="F21" s="25" t="s">
@@ -1047,13 +1060,13 @@
       <c r="B22" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="30">
         <v>44201</v>
       </c>
       <c r="D22" s="25">
         <v>24</v>
       </c>
-      <c r="E22" s="31">
+      <c r="E22" s="30">
         <v>44201</v>
       </c>
       <c r="F22" s="25" t="s">
@@ -1084,13 +1097,13 @@
       <c r="B24" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="31">
+      <c r="C24" s="30">
         <v>44199</v>
       </c>
       <c r="D24" s="24">
         <v>1</v>
       </c>
-      <c r="E24" s="31">
+      <c r="E24" s="30">
         <v>44199</v>
       </c>
       <c r="F24" s="25" t="s">
@@ -1105,13 +1118,13 @@
       <c r="B25" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="31">
+      <c r="C25" s="30">
         <v>44200</v>
       </c>
       <c r="D25" s="24">
         <v>1</v>
       </c>
-      <c r="E25" s="31">
+      <c r="E25" s="30">
         <v>44200</v>
       </c>
       <c r="F25" s="25" t="s">
@@ -1123,7 +1136,7 @@
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="33" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="23">

</xml_diff>

<commit_message>
Actualización del cronograma 01/01/2021
</commit_message>
<xml_diff>
--- a/Desarrollo/comparape/SCPPN_CP.xlsx
+++ b/Desarrollo/comparape/SCPPN_CP.xlsx
@@ -339,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -431,6 +431,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -439,13 +447,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,7 +668,7 @@
   <dimension ref="B1:J997"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -687,34 +690,34 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
     </row>
     <row r="3" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
     </row>
     <row r="4" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -857,14 +860,14 @@
       <c r="J11" s="27"/>
     </row>
     <row r="12" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="40">
         <v>44193</v>
       </c>
       <c r="D12" s="36"/>
-      <c r="E12" s="44">
+      <c r="E12" s="40">
         <v>44195</v>
       </c>
       <c r="F12" s="36"/>
@@ -873,7 +876,7 @@
       </c>
     </row>
     <row r="13" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="41" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="35">
@@ -882,7 +885,7 @@
       <c r="D13" s="36">
         <v>5</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="42">
         <v>44197</v>
       </c>
       <c r="F13" s="36" t="s">
@@ -894,23 +897,23 @@
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="35">
         <v>44196</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="36">
         <v>5</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="42">
         <v>44197</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="26">
-        <v>0</v>
+      <c r="G14" s="37">
+        <v>1</v>
       </c>
       <c r="I14" s="3"/>
     </row>

</xml_diff>

<commit_message>
Actualización del cronograma 03/01/2021
</commit_message>
<xml_diff>
--- a/Desarrollo/comparape/SCPPN_CP.xlsx
+++ b/Desarrollo/comparape/SCPPN_CP.xlsx
@@ -27,9 +27,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Proyecto: ComparaPe</t>
-  </si>
-  <si>
-    <t>Fecha de Inicio: 19/10/2020</t>
   </si>
   <si>
     <t>Actividad</t>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>Fecha de Termino: 08/01/2021</t>
+  </si>
+  <si>
+    <t>Fecha de Inicio: 21/10/2020</t>
   </si>
 </sst>
 </file>
@@ -339,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -413,9 +413,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -439,6 +436,9 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -447,9 +447,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,7 +665,7 @@
   <dimension ref="B1:J997"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -701,7 +698,7 @@
     </row>
     <row r="3" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B3" s="43" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C3" s="44"/>
       <c r="D3" s="44"/>
@@ -711,7 +708,7 @@
     </row>
     <row r="4" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" s="45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
@@ -722,27 +719,27 @@
     </row>
     <row r="5" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="10">
         <v>44125</v>
@@ -754,7 +751,7 @@
         <v>44128</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="12">
         <v>1</v>
@@ -763,7 +760,7 @@
     </row>
     <row r="7" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B7" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="10">
         <v>44125</v>
@@ -775,7 +772,7 @@
         <v>44125</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="15">
         <v>1</v>
@@ -784,7 +781,7 @@
     </row>
     <row r="8" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B8" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="18"/>
@@ -796,7 +793,7 @@
     </row>
     <row r="9" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B9" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="10">
         <v>44193</v>
@@ -808,7 +805,7 @@
         <v>44193</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="19">
         <v>1</v>
@@ -816,168 +813,168 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="34">
+        <v>44193</v>
+      </c>
+      <c r="D10" s="35">
+        <v>1</v>
+      </c>
+      <c r="E10" s="34">
+        <v>44194</v>
+      </c>
+      <c r="F10" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="35">
-        <v>44193</v>
-      </c>
-      <c r="D10" s="36">
-        <v>1</v>
-      </c>
-      <c r="E10" s="35">
-        <v>44194</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="37">
+      <c r="G10" s="36">
         <v>1</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="27"/>
     </row>
     <row r="11" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="35">
+      <c r="B11" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="34">
         <v>44195</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D11" s="35">
         <v>1</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="34">
         <v>44195</v>
       </c>
-      <c r="F11" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="37">
+      <c r="F11" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="36">
         <v>1</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="27"/>
     </row>
     <row r="12" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="39">
+        <v>44193</v>
+      </c>
+      <c r="D12" s="35"/>
+      <c r="E12" s="39">
+        <v>44195</v>
+      </c>
+      <c r="F12" s="35"/>
+      <c r="G12" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B13" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="40">
-        <v>44193</v>
-      </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="40">
+      <c r="C13" s="34">
+        <v>44196</v>
+      </c>
+      <c r="D13" s="35">
+        <v>5</v>
+      </c>
+      <c r="E13" s="41">
+        <v>44197</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="36">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="34">
+        <v>44196</v>
+      </c>
+      <c r="D14" s="35">
+        <v>5</v>
+      </c>
+      <c r="E14" s="41">
+        <v>44197</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="36">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B15" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="41">
+        <v>44197</v>
+      </c>
+      <c r="D15" s="35">
+        <v>3</v>
+      </c>
+      <c r="E15" s="41">
+        <v>44198</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="36">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="34">
         <v>44195</v>
       </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37">
+      <c r="D16" s="35">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B13" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="35">
+      <c r="E16" s="34">
+        <v>44195</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="36">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="39">
         <v>44196</v>
       </c>
-      <c r="D13" s="36">
-        <v>5</v>
-      </c>
-      <c r="E13" s="42">
-        <v>44197</v>
-      </c>
-      <c r="F13" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="37">
+      <c r="D17" s="35"/>
+      <c r="E17" s="39">
+        <v>44198</v>
+      </c>
+      <c r="F17" s="35"/>
+      <c r="G17" s="36">
         <v>1</v>
       </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="35">
-        <v>44196</v>
-      </c>
-      <c r="D14" s="36">
-        <v>5</v>
-      </c>
-      <c r="E14" s="42">
-        <v>44197</v>
-      </c>
-      <c r="F14" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="37">
-        <v>1</v>
-      </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="30">
-        <v>44197</v>
-      </c>
-      <c r="D15" s="25">
-        <v>3</v>
-      </c>
-      <c r="E15" s="30">
-        <v>44198</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="26">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="23">
-        <v>44195</v>
-      </c>
-      <c r="D16" s="24">
-        <v>1</v>
-      </c>
-      <c r="E16" s="23">
-        <v>44195</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="26">
-        <v>0</v>
-      </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="28" t="s">
+    </row>
+    <row r="18" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="31" t="s">
         <v>24</v>
-      </c>
-      <c r="C17" s="29">
-        <v>44196</v>
-      </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="29">
-        <v>44198</v>
-      </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="32" t="s">
-        <v>25</v>
       </c>
       <c r="C18" s="30">
         <v>44199</v>
@@ -989,7 +986,7 @@
         <v>44200</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18" s="26">
         <v>0</v>
@@ -998,7 +995,7 @@
     </row>
     <row r="19" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="30">
         <v>44199</v>
@@ -1010,16 +1007,16 @@
         <v>44200</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G19" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="32" t="s">
-        <v>28</v>
+      <c r="B20" s="31" t="s">
+        <v>27</v>
       </c>
       <c r="C20" s="30">
         <v>44200</v>
@@ -1031,16 +1028,16 @@
         <v>44201</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G20" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="30">
         <v>44200</v>
@@ -1052,7 +1049,7 @@
         <v>44200</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G21" s="26">
         <v>0</v>
@@ -1061,7 +1058,7 @@
     </row>
     <row r="22" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="30">
         <v>44201</v>
@@ -1073,7 +1070,7 @@
         <v>44201</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G22" s="26">
         <v>0</v>
@@ -1082,7 +1079,7 @@
     </row>
     <row r="23" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="29">
         <v>44199</v>
@@ -1098,7 +1095,7 @@
     </row>
     <row r="24" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="30">
         <v>44199</v>
@@ -1110,7 +1107,7 @@
         <v>44199</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G24" s="26">
         <v>0</v>
@@ -1119,7 +1116,7 @@
     </row>
     <row r="25" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="30">
         <v>44200</v>
@@ -1131,7 +1128,7 @@
         <v>44200</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G25" s="26">
         <v>0</v>
@@ -1139,8 +1136,8 @@
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="33" t="s">
-        <v>34</v>
+      <c r="B26" s="32" t="s">
+        <v>33</v>
       </c>
       <c r="C26" s="23">
         <v>44204</v>
@@ -1152,7 +1149,7 @@
         <v>44204</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G26" s="26">
         <v>0</v>
@@ -1161,7 +1158,7 @@
     </row>
     <row r="27" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="29">
         <v>44202</v>

</xml_diff>

<commit_message>
Actualización del cronograma 05/01/2021
</commit_message>
<xml_diff>
--- a/Desarrollo/comparape/SCPPN_CP.xlsx
+++ b/Desarrollo/comparape/SCPPN_CP.xlsx
@@ -339,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -393,9 +393,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -413,7 +410,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -439,6 +435,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -664,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -687,34 +684,34 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
     </row>
     <row r="3" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -745,7 +742,7 @@
         <v>44125</v>
       </c>
       <c r="D6" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="10">
         <v>44128</v>
@@ -766,7 +763,7 @@
         <v>44125</v>
       </c>
       <c r="D7" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="10">
         <v>44125</v>
@@ -813,303 +810,303 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="32">
         <v>44193</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="33">
+        <v>2</v>
+      </c>
+      <c r="E10" s="32">
+        <v>44194</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="34">
         <v>1</v>
       </c>
-      <c r="E10" s="34">
-        <v>44194</v>
-      </c>
-      <c r="F10" s="35" t="s">
+      <c r="I10" s="3"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B11" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="32">
+        <v>44195</v>
+      </c>
+      <c r="D11" s="33">
+        <v>1</v>
+      </c>
+      <c r="E11" s="32">
+        <v>44195</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="34">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="26"/>
+    </row>
+    <row r="12" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B12" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="37">
+        <v>44193</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="37">
+        <v>44195</v>
+      </c>
+      <c r="F12" s="33"/>
+      <c r="G12" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B13" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="32">
+        <v>44196</v>
+      </c>
+      <c r="D13" s="33">
+        <v>2</v>
+      </c>
+      <c r="E13" s="39">
+        <v>44197</v>
+      </c>
+      <c r="F13" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="34">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="32">
+        <v>44196</v>
+      </c>
+      <c r="D14" s="33">
+        <v>2</v>
+      </c>
+      <c r="E14" s="39">
+        <v>44197</v>
+      </c>
+      <c r="F14" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G14" s="34">
         <v>1</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="27"/>
-    </row>
-    <row r="11" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="34">
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B15" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="39">
+        <v>44197</v>
+      </c>
+      <c r="D15" s="33">
+        <v>2</v>
+      </c>
+      <c r="E15" s="39">
+        <v>44198</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="34">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="32">
         <v>44195</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D16" s="33">
         <v>1</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E16" s="32">
         <v>44195</v>
       </c>
-      <c r="F11" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="36">
+      <c r="F16" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="34">
         <v>1</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="27"/>
-    </row>
-    <row r="12" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B12" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="39">
-        <v>44193</v>
-      </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="39">
-        <v>44195</v>
-      </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36">
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="37">
+        <v>44196</v>
+      </c>
+      <c r="D17" s="33"/>
+      <c r="E17" s="37">
+        <v>44198</v>
+      </c>
+      <c r="F17" s="33"/>
+      <c r="G17" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B13" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="34">
-        <v>44196</v>
-      </c>
-      <c r="D13" s="35">
-        <v>5</v>
-      </c>
-      <c r="E13" s="41">
-        <v>44197</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="36">
+    <row r="18" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="39">
+        <v>44199</v>
+      </c>
+      <c r="D18" s="33">
+        <v>3</v>
+      </c>
+      <c r="E18" s="39">
+        <v>44201</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="34">
         <v>1</v>
       </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="34">
-        <v>44196</v>
-      </c>
-      <c r="D14" s="35">
-        <v>5</v>
-      </c>
-      <c r="E14" s="41">
-        <v>44197</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="36">
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="39">
+        <v>44199</v>
+      </c>
+      <c r="D19" s="33">
         <v>1</v>
       </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="41">
-        <v>44197</v>
-      </c>
-      <c r="D15" s="35">
-        <v>3</v>
-      </c>
-      <c r="E15" s="41">
-        <v>44198</v>
-      </c>
-      <c r="F15" s="35" t="s">
+      <c r="E19" s="39">
+        <v>44200</v>
+      </c>
+      <c r="F19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="36">
+      <c r="G19" s="34">
         <v>1</v>
       </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="34">
-        <v>44195</v>
-      </c>
-      <c r="D16" s="35">
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="39">
+        <v>44200</v>
+      </c>
+      <c r="D20" s="33">
+        <v>2</v>
+      </c>
+      <c r="E20" s="39">
+        <v>44201</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="34">
         <v>1</v>
       </c>
-      <c r="E16" s="34">
-        <v>44195</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="36">
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="39">
+        <v>44200</v>
+      </c>
+      <c r="D21" s="33">
+        <v>2</v>
+      </c>
+      <c r="E21" s="39">
+        <v>44201</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="34">
         <v>1</v>
       </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="39">
-        <v>44196</v>
-      </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="39">
-        <v>44198</v>
-      </c>
-      <c r="F17" s="35"/>
-      <c r="G17" s="36">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="39">
+        <v>44201</v>
+      </c>
+      <c r="D22" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="30">
+      <c r="E22" s="39">
+        <v>44201</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="34">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="37">
         <v>44199</v>
       </c>
-      <c r="D18" s="25">
-        <v>4</v>
-      </c>
-      <c r="E18" s="30">
-        <v>44200</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="26">
-        <v>0</v>
-      </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="30">
-        <v>44199</v>
-      </c>
-      <c r="D19" s="25">
-        <v>24</v>
-      </c>
-      <c r="E19" s="30">
-        <v>44200</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="26">
+      <c r="D23" s="33"/>
+      <c r="E23" s="37">
+        <v>44201</v>
+      </c>
+      <c r="F23" s="33"/>
+      <c r="G23" s="34">
         <v>1</v>
-      </c>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="30">
-        <v>44200</v>
-      </c>
-      <c r="D20" s="25">
-        <v>24</v>
-      </c>
-      <c r="E20" s="30">
-        <v>44201</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="26">
-        <v>1</v>
-      </c>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="30">
-        <v>44200</v>
-      </c>
-      <c r="D21" s="25">
-        <v>24</v>
-      </c>
-      <c r="E21" s="30">
-        <v>44200</v>
-      </c>
-      <c r="F21" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="26">
-        <v>0</v>
-      </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="30">
-        <v>44201</v>
-      </c>
-      <c r="D22" s="25">
-        <v>24</v>
-      </c>
-      <c r="E22" s="30">
-        <v>44201</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="26">
-        <v>0</v>
-      </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="29">
-        <v>44199</v>
-      </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="29">
-        <v>44201</v>
-      </c>
-      <c r="F23" s="25"/>
-      <c r="G23" s="26">
-        <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="30">
-        <v>44199</v>
-      </c>
-      <c r="D24" s="24">
+      <c r="C24" s="29">
+        <v>44202</v>
+      </c>
+      <c r="D24" s="23">
         <v>1</v>
       </c>
-      <c r="E24" s="30">
-        <v>44199</v>
-      </c>
-      <c r="F24" s="25" t="s">
+      <c r="E24" s="29">
+        <v>44202</v>
+      </c>
+      <c r="F24" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G24" s="26">
+      <c r="G24" s="25">
         <v>0</v>
       </c>
       <c r="I24" s="3"/>
@@ -1118,57 +1115,57 @@
       <c r="B25" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="30">
-        <v>44200</v>
-      </c>
-      <c r="D25" s="24">
+      <c r="C25" s="29">
+        <v>44203</v>
+      </c>
+      <c r="D25" s="23">
         <v>1</v>
       </c>
-      <c r="E25" s="30">
-        <v>44200</v>
-      </c>
-      <c r="F25" s="25" t="s">
+      <c r="E25" s="29">
+        <v>44203</v>
+      </c>
+      <c r="F25" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="26">
+      <c r="G25" s="25">
         <v>0</v>
       </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="23">
+      <c r="C26" s="29">
         <v>44204</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="23">
         <v>1</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="29">
         <v>44204</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F26" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="25">
         <v>0</v>
       </c>
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="29">
+      <c r="C27" s="28">
         <v>44202</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="29">
+      <c r="D27" s="24"/>
+      <c r="E27" s="28">
         <v>44204</v>
       </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
     </row>
     <row r="28" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="1"/>

</xml_diff>

<commit_message>
Actualización de cornograma final 08/01/2021
</commit_message>
<xml_diff>
--- a/Desarrollo/comparape/SCPPN_CP.xlsx
+++ b/Desarrollo/comparape/SCPPN_CP.xlsx
@@ -194,7 +194,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,12 +205,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCFE2F3"/>
         <bgColor rgb="FFCFE2F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -339,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -392,50 +386,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -661,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -684,34 +662,34 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
     </row>
     <row r="3" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -810,362 +788,363 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="24">
         <v>44193</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="25">
         <v>2</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="24">
         <v>44194</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="26">
         <v>1</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="26"/>
+      <c r="J10" s="22"/>
     </row>
     <row r="11" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="24">
         <v>44195</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="25">
         <v>1</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="24">
         <v>44195</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="26">
         <v>1</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="26"/>
+      <c r="J11" s="22"/>
     </row>
     <row r="12" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="29">
         <v>44193</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="37">
+      <c r="D12" s="25"/>
+      <c r="E12" s="29">
         <v>44195</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="34">
+      <c r="F12" s="25"/>
+      <c r="G12" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B13" s="38" t="s">
+    <row r="13" spans="2:10" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B13" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="24">
+        <v>44195</v>
+      </c>
+      <c r="D13" s="25">
+        <v>1</v>
+      </c>
+      <c r="E13" s="24">
+        <v>44195</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B14" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C14" s="24">
         <v>44196</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D14" s="25">
         <v>2</v>
       </c>
-      <c r="E13" s="39">
+      <c r="E14" s="31">
         <v>44197</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F14" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G14" s="26">
         <v>1</v>
       </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="40" t="s">
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C15" s="24">
         <v>44196</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D15" s="25">
         <v>2</v>
       </c>
-      <c r="E14" s="39">
+      <c r="E15" s="31">
         <v>44197</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F15" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G15" s="26">
         <v>1</v>
       </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="40" t="s">
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B16" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="39">
+      <c r="C16" s="31">
         <v>44197</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D16" s="25">
         <v>2</v>
       </c>
-      <c r="E15" s="39">
+      <c r="E16" s="31">
         <v>44198</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F16" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G16" s="26">
         <v>1</v>
       </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="32">
-        <v>44195</v>
-      </c>
-      <c r="D16" s="33">
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="29">
+        <v>44196</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="29">
+        <v>44198</v>
+      </c>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26">
         <v>1</v>
       </c>
-      <c r="E16" s="32">
-        <v>44195</v>
-      </c>
-      <c r="F16" s="33" t="s">
+    </row>
+    <row r="18" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="31">
+        <v>44199</v>
+      </c>
+      <c r="D18" s="25">
+        <v>3</v>
+      </c>
+      <c r="E18" s="31">
+        <v>44201</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="26">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="31">
+        <v>44199</v>
+      </c>
+      <c r="D19" s="25">
+        <v>1</v>
+      </c>
+      <c r="E19" s="31">
+        <v>44200</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="26">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="31">
+        <v>44200</v>
+      </c>
+      <c r="D20" s="25">
+        <v>2</v>
+      </c>
+      <c r="E20" s="31">
+        <v>44201</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="26">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="31">
+        <v>44200</v>
+      </c>
+      <c r="D21" s="25">
+        <v>2</v>
+      </c>
+      <c r="E21" s="31">
+        <v>44201</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="26">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="31">
+        <v>44201</v>
+      </c>
+      <c r="D22" s="25">
+        <v>1</v>
+      </c>
+      <c r="E22" s="31">
+        <v>44201</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="26">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="29">
+        <v>44199</v>
+      </c>
+      <c r="D23" s="25"/>
+      <c r="E23" s="29">
+        <v>44201</v>
+      </c>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="31">
+        <v>44202</v>
+      </c>
+      <c r="D24" s="25">
+        <v>1</v>
+      </c>
+      <c r="E24" s="31">
+        <v>44202</v>
+      </c>
+      <c r="F24" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G24" s="26">
         <v>1</v>
       </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="37">
-        <v>44196</v>
-      </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="37">
-        <v>44198</v>
-      </c>
-      <c r="F17" s="33"/>
-      <c r="G17" s="34">
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="31">
+        <v>44203</v>
+      </c>
+      <c r="D25" s="25">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="39">
-        <v>44199</v>
-      </c>
-      <c r="D18" s="33">
-        <v>3</v>
-      </c>
-      <c r="E18" s="39">
-        <v>44201</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="34">
+      <c r="E25" s="31">
+        <v>44203</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="26">
         <v>1</v>
       </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="39">
-        <v>44199</v>
-      </c>
-      <c r="D19" s="33">
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="31">
+        <v>44204</v>
+      </c>
+      <c r="D26" s="25">
         <v>1</v>
       </c>
-      <c r="E19" s="39">
-        <v>44200</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="34">
+      <c r="E26" s="31">
+        <v>44204</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="26">
         <v>1</v>
       </c>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="39">
-        <v>44200</v>
-      </c>
-      <c r="D20" s="33">
-        <v>2</v>
-      </c>
-      <c r="E20" s="39">
-        <v>44201</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="34">
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="29">
+        <v>44202</v>
+      </c>
+      <c r="D27" s="25"/>
+      <c r="E27" s="29">
+        <v>44204</v>
+      </c>
+      <c r="F27" s="25"/>
+      <c r="G27" s="26">
         <v>1</v>
       </c>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="39">
-        <v>44200</v>
-      </c>
-      <c r="D21" s="33">
-        <v>2</v>
-      </c>
-      <c r="E21" s="39">
-        <v>44201</v>
-      </c>
-      <c r="F21" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="34">
-        <v>1</v>
-      </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="39">
-        <v>44201</v>
-      </c>
-      <c r="D22" s="33">
-        <v>1</v>
-      </c>
-      <c r="E22" s="39">
-        <v>44201</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="34">
-        <v>1</v>
-      </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="37">
-        <v>44199</v>
-      </c>
-      <c r="D23" s="33"/>
-      <c r="E23" s="37">
-        <v>44201</v>
-      </c>
-      <c r="F23" s="33"/>
-      <c r="G23" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="29">
-        <v>44202</v>
-      </c>
-      <c r="D24" s="23">
-        <v>1</v>
-      </c>
-      <c r="E24" s="29">
-        <v>44202</v>
-      </c>
-      <c r="F24" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="25">
-        <v>0</v>
-      </c>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="29">
-        <v>44203</v>
-      </c>
-      <c r="D25" s="23">
-        <v>1</v>
-      </c>
-      <c r="E25" s="29">
-        <v>44203</v>
-      </c>
-      <c r="F25" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="25">
-        <v>0</v>
-      </c>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="29">
-        <v>44204</v>
-      </c>
-      <c r="D26" s="23">
-        <v>1</v>
-      </c>
-      <c r="E26" s="29">
-        <v>44204</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="25">
-        <v>0</v>
-      </c>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="28">
-        <v>44202</v>
-      </c>
-      <c r="D27" s="24"/>
-      <c r="E27" s="28">
-        <v>44204</v>
-      </c>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
     </row>
     <row r="28" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="1"/>

</xml_diff>